<commit_message>
- diary nachgeführt - scrum file aktualisiert
</commit_message>
<xml_diff>
--- a/doc/task06/Scrum_TeamYellow.xlsx
+++ b/doc/task06/Scrum_TeamYellow.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Surface_Faebu\OneDrive\BFH Share\Team\Team Gelb SOED\06_Task06\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Surface_Faebu\OneDrive\BFH Share\Team\Team Gelb SOED\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="236" documentId="11_00D15CF8CB76791963F5B1955475E5AAF0F2FE9E" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{94C9B5AB-2FAA-43F3-BD61-68D71BE86E6C}"/>
+  <xr:revisionPtr revIDLastSave="587" documentId="11_00D15CF8CB76791963F5B1955475E5AAF0F2FE9E" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{8851237A-3073-4200-A14E-CFDB3EBA3184}"/>
   <bookViews>
     <workbookView xWindow="383" yWindow="120" windowWidth="16485" windowHeight="9315" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="105">
   <si>
     <t>Name</t>
   </si>
@@ -121,27 +121,15 @@
     <t>Status</t>
   </si>
   <si>
-    <t>0h</t>
-  </si>
-  <si>
     <t>waiting</t>
   </si>
   <si>
-    <t>Patient</t>
-  </si>
-  <si>
-    <t>Der Anwender soll die Möglichkeit haben, Patienten zu verwalten (erfassen, mutieren, suchen)</t>
-  </si>
-  <si>
     <t>high</t>
   </si>
   <si>
     <t>Krankheitsverlauf</t>
   </si>
   <si>
-    <t>Der Anwender soll die Möglichkeit haben, Krankheitverläufe von Patienten zu verwalten (erstellen, mutieren, durchsuchen)</t>
-  </si>
-  <si>
     <t>medium</t>
   </si>
   <si>
@@ -181,15 +169,6 @@
     <t>Login</t>
   </si>
   <si>
-    <t>Person-Suchfunktion</t>
-  </si>
-  <si>
-    <t>Person-Erfassfunktion</t>
-  </si>
-  <si>
-    <t>Person-Editierfunktion</t>
-  </si>
-  <si>
     <t>Reserve</t>
   </si>
   <si>
@@ -206,6 +185,159 @@
   </si>
   <si>
     <t>Remaining Ressources</t>
+  </si>
+  <si>
+    <t>Kontakte</t>
+  </si>
+  <si>
+    <t>FileUp- und Download</t>
+  </si>
+  <si>
+    <t>Der Anwender soll die Möglichkeit haben, Patienten zu verwalten (erfassen, mutieren, suchen). Er soll ausserdem eine Liste von Patienten zur Verfügung haben, die er filtern und durchsuchen kann.</t>
+  </si>
+  <si>
+    <t>Der Anwender soll die Möglichkeit haben, Krankheitverläufe von Patienten zu verwalten (erstellen, mutieren, durchsuchen). Er soll ausserdem eine Liste von Medikamenten zur Verfügung haben, die er filtern und durchsuchen kann.</t>
+  </si>
+  <si>
+    <t>Der Anwender soll die Möglichkeit haben, Kontakte für den Patienten zu verwalten (erfassen, mutieren, suchen). Es sollen jeweils ein Arzt und eine Versicherung pro Patient und mehrere Angehörige erfasst werden. Kontakte sollen mehreren Patienten zugewiesen werden können.</t>
+  </si>
+  <si>
+    <t>Medikation</t>
+  </si>
+  <si>
+    <t>Der Anwender soll die Möglichkeit haben für einen Patienten eine Medikation zu Erfassen. Diese beinhaltet eine Dosis sowie einen Zeitraum wo sie aktiv ist.</t>
+  </si>
+  <si>
+    <t>Benutzerverwaltung</t>
+  </si>
+  <si>
+    <t>Der Anwender soll die Möglichkeit haben, Files hoch- und runterzuladen (z.B Dokumente von Arzt und Versicherung)</t>
+  </si>
+  <si>
+    <t>Projekt-Setup Vaadin</t>
+  </si>
+  <si>
+    <t>Ein neuer Benutzer (freischaffende Spitex-Pflegeperson) soll sich registrieren und dann einloggen, sowie sein Profil bearbeiten können.</t>
+  </si>
+  <si>
+    <t>Registration</t>
+  </si>
+  <si>
+    <t>Eclipse einrichten und ein Vaadin Projekt erstellen auf dem SVN Server</t>
+  </si>
+  <si>
+    <t>Projektsetup so wie erstellen des globalen CSS</t>
+  </si>
+  <si>
+    <t>Startseite (Personen-Suche)</t>
+  </si>
+  <si>
+    <t>Grundeinstellungen</t>
+  </si>
+  <si>
+    <t>Entwicklungsumgebung einrichten</t>
+  </si>
+  <si>
+    <t>Menubar Header implementieren</t>
+  </si>
+  <si>
+    <t>Der Benutzer soll sich sein Profil bearbeiten können.</t>
+  </si>
+  <si>
+    <t>Sollten 210h sein</t>
+  </si>
+  <si>
+    <t>Patientenverwaltung</t>
+  </si>
+  <si>
+    <t>DB - Server</t>
+  </si>
+  <si>
+    <t>MY SQL Server aufsetzen</t>
+  </si>
+  <si>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>DB - Schema</t>
+  </si>
+  <si>
+    <t>Datenbankschema planen</t>
+  </si>
+  <si>
+    <t>Datenbankschema umsetzen</t>
+  </si>
+  <si>
+    <t>DB - Einträge</t>
+  </si>
+  <si>
+    <t>Testeinträge erfassen</t>
+  </si>
+  <si>
+    <t>DB - Dok</t>
+  </si>
+  <si>
+    <t>Alle Einträge dokumentieren</t>
+  </si>
+  <si>
+    <t>Datenbankschema in Datei speichern</t>
+  </si>
+  <si>
+    <t>Profil bearbeiten</t>
+  </si>
+  <si>
+    <t>Implementieren der Patientenübersicht, die der Benutzer sieht, sobald er sich in der Software einloggt. Es wird eine Liste dargestellt, welche gefiltert werden kann.</t>
+  </si>
+  <si>
+    <t>1.3.1</t>
+  </si>
+  <si>
+    <t>1.3.2</t>
+  </si>
+  <si>
+    <t>1.3.3</t>
+  </si>
+  <si>
+    <t>1.3.4</t>
+  </si>
+  <si>
+    <t>1.3.5</t>
+  </si>
+  <si>
+    <t>1.3.6</t>
+  </si>
+  <si>
+    <t>Implementieren der Menubar der App. Rechts oben soll der aktuell eingeloggte Benutzer angezeigt werden. Der Benutzer soll sein Profil bearbeiten können +  ausloggen</t>
+  </si>
+  <si>
+    <t>2.3</t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>2.4</t>
+  </si>
+  <si>
+    <t>Patient-Suchfunktion</t>
+  </si>
+  <si>
+    <t>Implementieren der Patientensuchfunktion (Suchen und Filtern nach Patientenattributen)</t>
+  </si>
+  <si>
+    <t>in Progress</t>
+  </si>
+  <si>
+    <t>Philip Köfer</t>
+  </si>
+  <si>
+    <t>Implementieren der Login-Seite</t>
+  </si>
+  <si>
+    <t>Implementieren der Registration der Spitex-Person</t>
+  </si>
+  <si>
+    <t>DB - Backup</t>
   </si>
 </sst>
 </file>
@@ -389,11 +521,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -430,12 +559,32 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1795,120 +1944,120 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.73046875" customWidth="1"/>
-    <col min="2" max="2" width="18.59765625" customWidth="1"/>
-    <col min="3" max="3" width="14.59765625" customWidth="1"/>
+    <col min="1" max="1" width="19.796875" customWidth="1"/>
+    <col min="2" max="2" width="18.53125" customWidth="1"/>
+    <col min="3" max="3" width="14.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" ht="19.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="19.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="13"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="14"/>
+      <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="10"/>
+      <c r="C10" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1918,151 +2067,264 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="3.86328125" customWidth="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39" customWidth="1"/>
-    <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="11.73046875" customWidth="1"/>
-    <col min="6" max="6" width="13.1328125" customWidth="1"/>
-    <col min="7" max="7" width="10.1328125" customWidth="1"/>
-    <col min="8" max="8" width="14.3984375" customWidth="1"/>
+    <col min="1" max="1" width="3.86328125" style="20" customWidth="1"/>
+    <col min="2" max="2" width="24.1328125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="63.53125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="9" style="20" customWidth="1"/>
+    <col min="5" max="5" width="11.796875" style="20" customWidth="1"/>
+    <col min="6" max="6" width="21.86328125" style="20" customWidth="1"/>
+    <col min="7" max="7" width="10.1328125" style="20" customWidth="1"/>
+    <col min="8" max="8" width="14.46484375" style="20" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="16" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A2" s="1">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2" s="20">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="1">
-        <v>63</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="B2" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="20">
+        <v>0</v>
+      </c>
+      <c r="H2" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="20">
+        <v>2</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="20" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3">
-        <v>63</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="E3" s="20">
+        <v>6</v>
+      </c>
+      <c r="G3" s="20">
+        <v>0</v>
+      </c>
+      <c r="H3" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:8" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="1">
+        <v>63</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="57" x14ac:dyDescent="0.45">
+      <c r="A5" s="21">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="20">
+        <v>35</v>
+      </c>
+      <c r="G5" s="20">
+        <v>0</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="20">
+        <v>63</v>
+      </c>
+      <c r="G6" s="20">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="21">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="20">
+        <v>0</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="20">
+        <v>35</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="20">
+        <v>7</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4">
-        <v>70</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="D10" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="20">
+        <v>7</v>
+      </c>
+      <c r="G10" s="20">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5">
-        <v>14</v>
-      </c>
-      <c r="G5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B6" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19">
-        <f>SUM(E2:E5)</f>
-        <v>210</v>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B11" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24">
+        <f>SUM(E2:E10)</f>
+        <v>216</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2073,243 +2335,564 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K9"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="4.86328125" customWidth="1"/>
+    <col min="1" max="1" width="10.1328125" style="27" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="19.86328125" customWidth="1"/>
-    <col min="4" max="4" width="13.86328125" customWidth="1"/>
-    <col min="5" max="5" width="11.53125" customWidth="1"/>
-    <col min="6" max="6" width="9.19921875" customWidth="1"/>
-    <col min="7" max="7" width="8.265625" customWidth="1"/>
-    <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="9.1328125" customWidth="1"/>
-    <col min="10" max="10" width="7.1328125" customWidth="1"/>
-    <col min="11" max="11" width="15.1328125" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="58.86328125" customWidth="1"/>
+    <col min="5" max="5" width="13.86328125" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.86328125" customWidth="1"/>
+    <col min="8" max="8" width="8.19921875" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
+    <col min="10" max="10" width="9.1328125" customWidth="1"/>
+    <col min="11" max="11" width="7.1328125" customWidth="1"/>
+    <col min="12" max="12" width="15.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="26">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B2" s="20">
+        <v>1</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="20">
+        <v>4</v>
+      </c>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20">
+        <v>4</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A3" s="26">
+        <v>1.2</v>
+      </c>
+      <c r="B3" s="20">
+        <v>1</v>
+      </c>
+      <c r="C3" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A2">
-        <v>0.1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2">
-        <v>16</v>
-      </c>
-      <c r="I2">
-        <v>16</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="D3" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="20" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A3">
-        <v>0.2</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H3">
-        <v>8</v>
-      </c>
-      <c r="I3">
-        <v>8</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A4">
-        <v>0.3</v>
+      <c r="I3" s="20">
+        <v>4</v>
+      </c>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A4" s="26" t="s">
+        <v>88</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
-      </c>
-      <c r="G4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4">
-        <v>4</v>
-      </c>
-      <c r="I4">
-        <v>4</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="H4" s="20" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A5">
-        <v>1.1000000000000001</v>
+      <c r="I4" s="20">
+        <v>2</v>
+      </c>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A5" s="26" t="s">
+        <v>89</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5">
-        <v>8</v>
-      </c>
-      <c r="I5">
-        <v>8</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="H5" s="20" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A6">
-        <v>1.2</v>
+      <c r="I5" s="20">
+        <v>2</v>
+      </c>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A6" s="26" t="s">
+        <v>90</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
-      </c>
-      <c r="G6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6">
-        <v>16</v>
-      </c>
-      <c r="I6">
-        <v>16</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="H6" s="20" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A7">
-        <v>1.3</v>
+      <c r="I6" s="20">
+        <v>2</v>
+      </c>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A7" s="26" t="s">
+        <v>91</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7">
+        <v>81</v>
+      </c>
+      <c r="D7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="20">
+        <v>2</v>
+      </c>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A8" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="20">
+        <v>2</v>
+      </c>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A9" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" t="s">
+        <v>85</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="20">
+        <v>2</v>
+      </c>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A10" s="26">
+        <v>2.1</v>
+      </c>
+      <c r="B10" s="20">
+        <v>1</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="20">
+        <v>4</v>
+      </c>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20">
+        <v>0</v>
+      </c>
+      <c r="L10" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A11" s="26">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B11" s="20">
+        <v>1</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" s="20">
         <v>8</v>
       </c>
-      <c r="I7">
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A12" s="26">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B12" s="20">
+        <v>1</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" s="20">
         <v>8</v>
       </c>
-      <c r="J7">
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A13" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="20">
+        <v>1</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" s="20">
+        <v>4</v>
+      </c>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A14" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="20">
+        <v>1</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="I14" s="20">
+        <v>8</v>
+      </c>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A15" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" s="20">
+        <v>1</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="I15" s="20">
+        <v>8</v>
+      </c>
+      <c r="J15" s="20">
+        <v>8</v>
+      </c>
+      <c r="K15" s="20">
         <v>0</v>
       </c>
-      <c r="K7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C8" t="s">
-        <v>55</v>
-      </c>
-      <c r="H8">
+      <c r="L15" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B16" s="20">
+        <v>1</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="I16" s="20">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A9" s="21"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="19">
-        <f>SUM(H2:H8)</f>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A17" s="28"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="17"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="17">
+        <f>SUM(I2:I16)</f>
         <v>63</v>
       </c>
+      <c r="J17" s="20"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J18" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2327,29 +2910,29 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.73046875" customWidth="1"/>
-    <col min="4" max="4" width="14.265625" customWidth="1"/>
+    <col min="3" max="3" width="14.796875" customWidth="1"/>
+    <col min="4" max="4" width="14.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>60</v>
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>42262</v>
       </c>
       <c r="C2">
@@ -2363,7 +2946,7 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>42263</v>
       </c>
       <c r="C3">

</xml_diff>